<commit_message>
Parameterized the regitser test
</commit_message>
<xml_diff>
--- a/src/config/data.xlsx
+++ b/src/config/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>TCID</t>
   </si>
@@ -46,6 +46,33 @@
   </si>
   <si>
     <t>Runmode</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Test Doc</t>
+  </si>
+  <si>
+    <t>testdoc11may@mailinator.com</t>
+  </si>
+  <si>
+    <t>Test Address</t>
+  </si>
+  <si>
+    <t>11 May</t>
   </si>
 </sst>
 </file>
@@ -90,9 +117,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -397,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -483,14 +520,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1245796545</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>